<commit_message>
- New template. Last time wasn't correct.
</commit_message>
<xml_diff>
--- a/WorkHoursTracker/WorkHoursTrackTemplate.xlsx
+++ b/WorkHoursTracker/WorkHoursTrackTemplate.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obadicb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simovicn\source\repos\WorkHoursTracker\WorkHoursTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D46F4C-2B4A-4836-9460-29FD21101A92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23270" windowHeight="12590"/>
+    <workbookView xWindow="-180" yWindow="1365" windowWidth="27405" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -92,22 +93,22 @@
     <t>* - Vacation / ** - Public holiday /  *** - Illness</t>
   </si>
   <si>
-    <t>EC</t>
+    <t>&lt;EmployeeID&gt;</t>
   </si>
   <si>
-    <t>Ime Prezime</t>
+    <t>&lt;FirstName_LastName&gt;</t>
   </si>
   <si>
-    <t>EMEA\username</t>
+    <t>&lt;Title&gt;</t>
   </si>
   <si>
-    <t>IT</t>
+    <t>&lt;Department&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
@@ -672,6 +673,111 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="23" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="22" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -692,119 +798,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="23" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="22" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="2"/>
-    <cellStyle name="Excel Built-in Normal" xfId="4"/>
+    <cellStyle name="Currency 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="TableStyleLight1" xfId="5"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="TableStyleLight1" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -847,7 +848,7 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -917,7 +918,7 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -987,7 +988,7 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1057,7 +1058,7 @@
         <xdr:cNvPr id="6" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1122,7 +1123,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1368,6 +1369,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1403,6 +1421,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1578,187 +1613,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="29" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="29" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="29" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" style="29" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" style="29" customWidth="1"/>
-    <col min="10" max="10" width="27.1796875" style="29" customWidth="1"/>
-    <col min="11" max="11" width="107.453125" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="29"/>
+    <col min="1" max="1" width="8.5703125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="107.42578125" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" s="32" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+    <row r="1" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:12" s="25" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="F2" s="33"/>
-    </row>
-    <row r="3" spans="2:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-    </row>
-    <row r="4" spans="2:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="31"/>
-    </row>
-    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-    </row>
-    <row r="6" spans="2:12" s="32" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="C2" s="24"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="2:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="2:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+    </row>
+    <row r="6" spans="2:12" s="25" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="61"/>
+      <c r="E6" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+    </row>
+    <row r="7" spans="2:12" s="25" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="32"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="2:12" s="25" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-    </row>
-    <row r="7" spans="2:12" s="32" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
-      <c r="H7" s="39"/>
-    </row>
-    <row r="8" spans="2:12" s="32" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="43" t="s">
+      <c r="D8" s="61"/>
+      <c r="E8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-    </row>
-    <row r="9" spans="2:12" s="32" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="H9" s="39"/>
-    </row>
-    <row r="10" spans="2:12" s="32" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+    </row>
+    <row r="9" spans="2:12" s="25" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="2:12" s="25" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="63">
         <v>44896</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="44" t="s">
+      <c r="D10" s="64"/>
+      <c r="E10" s="37" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="1">
         <f>NETWORKDAYS(C10, EOMONTH(C10,0))</f>
         <v>22</v>
       </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-    </row>
-    <row r="11" spans="2:12" s="32" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+    </row>
+    <row r="11" spans="2:12" s="25" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="47" t="s">
+      <c r="C12" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48" t="s">
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="48"/>
-      <c r="J12" s="49" t="s">
+      <c r="I12" s="59"/>
+      <c r="J12" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="50" t="s">
+      <c r="K12" s="51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="51" t="s">
+    <row r="13" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="56"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="51" t="s">
+      <c r="G13" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="52" t="s">
+      <c r="H13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="53" t="s">
+      <c r="I13" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
-    </row>
-    <row r="14" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
+    </row>
+    <row r="14" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="11">
         <f>IF(C10&lt;&gt;"",C10,"")</f>
         <v>44896</v>
@@ -1779,11 +1814,11 @@
         <f>IF(B14&lt;&gt;"",IF(((E14-D14)+(G14-F14))*24&gt;8,((E14-D14)+(G14-F14))*24-8,0),"")</f>
         <v>0</v>
       </c>
-      <c r="J14" s="62"/>
+      <c r="J14" s="44"/>
       <c r="K14" s="17"/>
-      <c r="L14" s="54"/>
-    </row>
-    <row r="15" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="41"/>
+    </row>
+    <row r="15" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13">
         <f>IFERROR(IF(MONTH($C$10)=MONTH(B14+1),B14+1,""),"")</f>
         <v>44897</v>
@@ -1804,10 +1839,10 @@
         <f t="shared" ref="I15:I44" si="2">IF(B15&lt;&gt;"",IF(((E15-D15)+(G15-F15))*24&gt;8,((E15-D15)+(G15-F15))*24-8,0),"")</f>
         <v>0</v>
       </c>
-      <c r="J15" s="62"/>
+      <c r="J15" s="44"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13">
         <f t="shared" ref="B16:B44" si="3">IFERROR(IF(MONTH($C$10)=MONTH(B15+1),B15+1,""),"")</f>
         <v>44898</v>
@@ -1828,10 +1863,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="62"/>
+      <c r="J16" s="44"/>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="13">
         <f t="shared" si="3"/>
         <v>44899</v>
@@ -1852,10 +1887,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="62"/>
+      <c r="J17" s="44"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="13">
         <f t="shared" si="3"/>
         <v>44900</v>
@@ -1876,10 +1911,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J18" s="62"/>
+      <c r="J18" s="44"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13">
         <f t="shared" si="3"/>
         <v>44901</v>
@@ -1900,10 +1935,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J19" s="62"/>
+      <c r="J19" s="44"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13">
         <f t="shared" si="3"/>
         <v>44902</v>
@@ -1924,10 +1959,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J20" s="62"/>
+      <c r="J20" s="44"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13">
         <f t="shared" si="3"/>
         <v>44903</v>
@@ -1948,10 +1983,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J21" s="62"/>
+      <c r="J21" s="44"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13">
         <f t="shared" si="3"/>
         <v>44904</v>
@@ -1972,11 +2007,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="62"/>
+      <c r="J22" s="44"/>
       <c r="K22" s="19"/>
-      <c r="L22" s="55"/>
-    </row>
-    <row r="23" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="42"/>
+    </row>
+    <row r="23" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="13">
         <f t="shared" si="3"/>
         <v>44905</v>
@@ -1997,10 +2032,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="62"/>
+      <c r="J23" s="44"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13">
         <f t="shared" si="3"/>
         <v>44906</v>
@@ -2021,10 +2056,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J24" s="62"/>
+      <c r="J24" s="44"/>
       <c r="K24" s="18"/>
     </row>
-    <row r="25" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="13">
         <f t="shared" si="3"/>
         <v>44907</v>
@@ -2045,11 +2080,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="62"/>
+      <c r="J25" s="44"/>
       <c r="K25" s="18"/>
-      <c r="L25" s="34"/>
-    </row>
-    <row r="26" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="27"/>
+    </row>
+    <row r="26" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13">
         <f t="shared" si="3"/>
         <v>44908</v>
@@ -2070,10 +2105,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J26" s="62"/>
+      <c r="J26" s="44"/>
       <c r="K26" s="18"/>
     </row>
-    <row r="27" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13">
         <f t="shared" si="3"/>
         <v>44909</v>
@@ -2094,10 +2129,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="62"/>
+      <c r="J27" s="44"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13">
         <f t="shared" si="3"/>
         <v>44910</v>
@@ -2118,10 +2153,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="62"/>
+      <c r="J28" s="44"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13">
         <f t="shared" si="3"/>
         <v>44911</v>
@@ -2142,10 +2177,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="62"/>
+      <c r="J29" s="44"/>
       <c r="K29" s="18"/>
     </row>
-    <row r="30" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="13">
         <f t="shared" si="3"/>
         <v>44912</v>
@@ -2166,11 +2201,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J30" s="62"/>
+      <c r="J30" s="44"/>
       <c r="K30" s="18"/>
-      <c r="L30" s="55"/>
-    </row>
-    <row r="31" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L30" s="42"/>
+    </row>
+    <row r="31" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="13">
         <f t="shared" si="3"/>
         <v>44913</v>
@@ -2191,10 +2226,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J31" s="62"/>
+      <c r="J31" s="44"/>
       <c r="K31" s="18"/>
     </row>
-    <row r="32" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="13">
         <f t="shared" si="3"/>
         <v>44914</v>
@@ -2215,10 +2250,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J32" s="62"/>
+      <c r="J32" s="44"/>
       <c r="K32" s="18"/>
     </row>
-    <row r="33" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="13">
         <f t="shared" si="3"/>
         <v>44915</v>
@@ -2239,10 +2274,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J33" s="62"/>
+      <c r="J33" s="44"/>
       <c r="K33" s="18"/>
     </row>
-    <row r="34" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="13">
         <f t="shared" si="3"/>
         <v>44916</v>
@@ -2263,10 +2298,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J34" s="62"/>
+      <c r="J34" s="44"/>
       <c r="K34" s="18"/>
     </row>
-    <row r="35" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="13">
         <f t="shared" si="3"/>
         <v>44917</v>
@@ -2287,10 +2322,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J35" s="62"/>
+      <c r="J35" s="44"/>
       <c r="K35" s="18"/>
     </row>
-    <row r="36" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="13">
         <f t="shared" si="3"/>
         <v>44918</v>
@@ -2311,10 +2346,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J36" s="62"/>
+      <c r="J36" s="44"/>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="13">
         <f t="shared" si="3"/>
         <v>44919</v>
@@ -2335,10 +2370,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J37" s="62"/>
+      <c r="J37" s="44"/>
       <c r="K37" s="21"/>
     </row>
-    <row r="38" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="13">
         <f t="shared" si="3"/>
         <v>44920</v>
@@ -2359,10 +2394,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J38" s="62"/>
+      <c r="J38" s="44"/>
       <c r="K38" s="21"/>
     </row>
-    <row r="39" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="13">
         <f t="shared" si="3"/>
         <v>44921</v>
@@ -2383,10 +2418,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J39" s="62"/>
+      <c r="J39" s="44"/>
       <c r="K39" s="21"/>
     </row>
-    <row r="40" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="13">
         <f t="shared" si="3"/>
         <v>44922</v>
@@ -2407,10 +2442,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J40" s="62"/>
+      <c r="J40" s="44"/>
       <c r="K40" s="18"/>
     </row>
-    <row r="41" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="13">
         <f t="shared" si="3"/>
         <v>44923</v>
@@ -2431,10 +2466,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J41" s="62"/>
+      <c r="J41" s="44"/>
       <c r="K41" s="18"/>
     </row>
-    <row r="42" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13">
         <f t="shared" si="3"/>
         <v>44924</v>
@@ -2455,10 +2490,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J42" s="62"/>
+      <c r="J42" s="44"/>
       <c r="K42" s="21"/>
     </row>
-    <row r="43" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="13">
         <f t="shared" si="3"/>
         <v>44925</v>
@@ -2479,10 +2514,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J43" s="63"/>
+      <c r="J43" s="45"/>
       <c r="K43" s="21"/>
     </row>
-    <row r="44" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="13">
         <f t="shared" si="3"/>
         <v>44926</v>
@@ -2503,18 +2538,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J44" s="64"/>
+      <c r="J44" s="46"/>
       <c r="K44" s="18"/>
     </row>
-    <row r="45" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="56" t="s">
+    <row r="45" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
       <c r="H45" s="3">
         <f>SUM(H14:H44)</f>
         <v>0</v>
@@ -2526,69 +2561,74 @@
       <c r="J45" s="5"/>
       <c r="K45" s="6"/>
     </row>
-    <row r="46" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
+    <row r="46" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
       <c r="J46" s="8"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="2:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
+    <row r="47" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
       <c r="J47" s="8"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="59" t="s">
+    <row r="48" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="27">
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="48">
         <f>H45+I45</f>
         <v>0</v>
       </c>
-      <c r="I48" s="27"/>
+      <c r="I48" s="48"/>
       <c r="J48" s="9"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="60"/>
-      <c r="B49" s="61" t="s">
+    <row r="49" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="43"/>
+      <c r="B49" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="61"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="60"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="60"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="43"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="43"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="MkYgxxml9EfHjhb3/eVzaUl3zxq1pk3udoSdCQyJ6cXd2LgIwYSlKQgDUAUPy4dztdDzFhavuk1PL5EjVxLfDA==" saltValue="zr3HgcZx5H5dRve8MXv7Vg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="B49:I49"/>
@@ -2603,11 +2643,6 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <conditionalFormatting sqref="K14:K44">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -2615,15 +2650,15 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Input" error="Please enter valid date from 1/1/2009 - 12/31/2025" sqref="C10:D10">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Input" error="Please enter valid date from 1/1/2009 - 12/31/2025" sqref="C10:D10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>39814</formula1>
       <formula2>46022</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please enter valid number from 1 - 31" sqref="K10">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please enter valid number from 1 - 31" sqref="K10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>31</formula2>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please enter time with format between 0:00 and 23:59." sqref="D14:G44">
+    <dataValidation type="time" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data Entry" error="Please enter time with format between 0:00 and 23:59." sqref="D14:G44" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>